<commit_message>
data updates October release
</commit_message>
<xml_diff>
--- a/static/download/2023/RP3_APT_ATFM_ARR_2023_Jan_Sep.xlsx
+++ b/static/download/2023/RP3_APT_ATFM_ARR_2023_Jan_Sep.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhegendo\Downloads\10-release-20231011T121513Z-001\10-release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhegendo\Downloads\10-release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580901B0-5933-44F7-AFDD-9742620CA701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD05D82-B8C4-40D8-A88D-CCF560639E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId6"/>
+    <pivotCache cacheId="21" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1360,106 +1360,89 @@
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFF3F3F3"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2152,7 +2135,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="HEGENDORFER Holger" refreshedDate="45210.594888888889" refreshedVersion="8" recordCount="145" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="HEGENDORFER Holger" refreshedDate="45215.714365624997" refreshedVersion="8" recordCount="145" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:F150" sheet="APT_ATFM_APT"/>
   </cacheSource>
@@ -3374,7 +3357,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="APT_ATFM_LOC" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" rowGrandTotals="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="APT_ATFM_LOC" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" rowGrandTotals="0" compact="0" compactData="0">
   <location ref="A5:D29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField name="State" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
@@ -5623,7 +5606,7 @@
   <dimension ref="A1:F530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>